<commit_message>
organized the project, revised metadata creation, added data query module, added a function for fundumental diagram (FD) creation
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,35 +441,40 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>route</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>mile_start</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>mile_end</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>weekend</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>direction</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>start_date</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>end_date</t>
         </is>
@@ -481,38 +486,43 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-01-01_2016-01-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Decreasing_0_190_MoTuWeThFr_2016-01-01_2016-01-31.xlsx</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>Decreasing</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>2016-01-01</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>2016-01-31</t>
         </is>
@@ -524,40 +534,45 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>005_Decreasing_0_190_MoTuWeThFr_2016-03-01_2016-03-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Decreasing_0_190_MoTuWeThFr_2016-02-01_2016-02-29.xlsx</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr">
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Decreasing</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2016-03-01</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2016-03-31</t>
+          <t>2016-02-01</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2016-02-29</t>
         </is>
       </c>
     </row>
@@ -567,40 +582,45 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>005_Decreasing_0_190_MoTuWeThFr_2016-02-01_2016-02-29</t>
+          <t>./data/DriveNet/averaged daily data/005_Decreasing_0_190_MoTuWeThFr_2016-03-01_2016-03-31.xlsx</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="inlineStr">
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>Decreasing</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2016-02-01</t>
-        </is>
-      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2016-02-29</t>
+          <t>2016-03-01</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2016-03-31</t>
         </is>
       </c>
     </row>
@@ -610,40 +630,45 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>005_Decreasing_0_190_MoTuWeThFr_2016-08-01_2016-08-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Decreasing_0_190_MoTuWeThFr_2016-04-01_2016-04-30.xlsx</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="inlineStr">
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>Decreasing</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2016-08-01</t>
-        </is>
-      </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2016-08-31</t>
+          <t>2016-04-01</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2016-04-30</t>
         </is>
       </c>
     </row>
@@ -653,40 +678,45 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-11-01_2016-11-30</t>
+          <t>./data/DriveNet/averaged daily data/005_Decreasing_0_190_MoTuWeThFr_2016-05-01_2016-05-31.xlsx</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2016-11-01</t>
+          <t>Decreasing</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2016-11-30</t>
+          <t>2016-05-01</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2016-05-31</t>
         </is>
       </c>
     </row>
@@ -696,40 +726,45 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>005_Decreasing_0_190_MoTuWeThFr_2016-04-01_2016-04-30</t>
+          <t>./data/DriveNet/averaged daily data/005_Decreasing_0_190_MoTuWeThFr_2016-06-01_2016-06-30.xlsx</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="inlineStr">
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>Decreasing</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>2016-04-01</t>
-        </is>
-      </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2016-04-30</t>
+          <t>2016-06-01</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2016-06-30</t>
         </is>
       </c>
     </row>
@@ -739,40 +774,45 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-06-01_2016-06-30</t>
+          <t>./data/DriveNet/averaged daily data/005_Decreasing_0_190_MoTuWeThFr_2016-07-01_2016-07-31.xlsx</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2016-06-01</t>
+          <t>Decreasing</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2016-06-30</t>
+          <t>2016-07-01</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2016-07-31</t>
         </is>
       </c>
     </row>
@@ -782,40 +822,45 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-09-01_2016-09-30</t>
+          <t>./data/DriveNet/averaged daily data/005_Decreasing_0_190_MoTuWeThFr_2016-08-01_2016-08-31.xlsx</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2016-09-01</t>
+          <t>Decreasing</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2016-09-30</t>
+          <t>2016-08-01</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2016-08-31</t>
         </is>
       </c>
     </row>
@@ -825,40 +870,45 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-12-01_2016-12-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Decreasing_0_190_MoTuWeThFr_2016-09-01_2016-09-30.xlsx</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2016-12-01</t>
+          <t>Decreasing</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2016-12-31</t>
+          <t>2016-09-01</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2016-09-30</t>
         </is>
       </c>
     </row>
@@ -868,40 +918,45 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>005_Decreasing_0_190_MoTuWeThFr_2016-07-01_2016-07-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Decreasing_0_190_MoTuWeThFr_2016-10-01_2016-10-31.xlsx</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" t="inlineStr">
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>Decreasing</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>2016-07-01</t>
-        </is>
-      </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2016-07-31</t>
+          <t>2016-10-01</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>2016-10-31</t>
         </is>
       </c>
     </row>
@@ -911,40 +966,45 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-05-01_2016-05-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Decreasing_0_190_MoTuWeThFr_2016-11-01_2016-11-30.xlsx</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2016-05-01</t>
+          <t>Decreasing</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2016-05-31</t>
+          <t>2016-11-01</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>2016-11-30</t>
         </is>
       </c>
     </row>
@@ -954,40 +1014,45 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>005_Decreasing_0_190_MoTuWeThFr_2016-10-01_2016-10-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Decreasing_0_190_MoTuWeThFr_2016-12-01_2016-12-31.xlsx</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" t="inlineStr">
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="inlineStr">
         <is>
           <t>Decreasing</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>2016-10-01</t>
-        </is>
-      </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2016-10-31</t>
+          <t>2016-12-01</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>2016-12-31</t>
         </is>
       </c>
     </row>
@@ -997,40 +1062,45 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>005_Decreasing_0_190_MoTuWeThFr_2016-06-01_2016-06-30</t>
+          <t>./data/DriveNet/averaged daily data/005_Increasing_0_190_MoTuWeThFr_2016-01-01_2016-01-31.xlsx</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Decreasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2016-06-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2016-06-30</t>
+          <t>2016-01-01</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>2016-01-31</t>
         </is>
       </c>
     </row>
@@ -1040,40 +1110,45 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>005_Decreasing_0_190_MoTuWeThFr_2016-11-01_2016-11-30</t>
+          <t>./data/DriveNet/averaged daily data/005_Increasing_0_190_MoTuWeThFr_2016-02-01_2016-02-29.xlsx</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Decreasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2016-11-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2016-11-30</t>
+          <t>2016-02-01</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>2016-02-29</t>
         </is>
       </c>
     </row>
@@ -1083,40 +1158,45 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-04-01_2016-04-30</t>
+          <t>./data/DriveNet/averaged daily data/005_Increasing_0_190_MoTuWeThFr_2016-03-01_2016-03-31.xlsx</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2016-04-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2016-04-30</t>
+          <t>2016-03-01</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>2016-03-31</t>
         </is>
       </c>
     </row>
@@ -1126,40 +1206,45 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-02-01_2016-02-29</t>
+          <t>./data/DriveNet/averaged daily data/005_Increasing_0_190_MoTuWeThFr_2016-04-01_2016-04-30.xlsx</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2016-02-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2016-02-29</t>
+          <t>2016-04-01</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>2016-04-30</t>
         </is>
       </c>
     </row>
@@ -1169,40 +1254,45 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-03-01_2016-03-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Increasing_0_190_MoTuWeThFr_2016-05-01_2016-05-31.xlsx</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2016-03-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2016-03-31</t>
+          <t>2016-05-01</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>2016-05-31</t>
         </is>
       </c>
     </row>
@@ -1212,40 +1302,45 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-08-01_2016-08-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Increasing_0_190_MoTuWeThFr_2016-06-01_2016-06-30.xlsx</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2016-08-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2016-08-31</t>
+          <t>2016-06-01</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>2016-06-30</t>
         </is>
       </c>
     </row>
@@ -1255,40 +1350,45 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>005_Decreasing_0_190_MoTuWeThFr_2016-01-01_2016-01-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Increasing_0_190_MoTuWeThFr_2016-07-01_2016-07-31.xlsx</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Decreasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2016-01-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2016-01-31</t>
+          <t>2016-07-01</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>2016-07-31</t>
         </is>
       </c>
     </row>
@@ -1298,40 +1398,45 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>005_Decreasing_0_190_MoTuWeThFr_2016-05-01_2016-05-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Increasing_0_190_MoTuWeThFr_2016-08-01_2016-08-31.xlsx</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Decreasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2016-05-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2016-05-31</t>
+          <t>2016-08-01</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>2016-08-31</t>
         </is>
       </c>
     </row>
@@ -1341,40 +1446,45 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-10-01_2016-10-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Increasing_0_190_MoTuWeThFr_2016-09-01_2016-09-30.xlsx</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F22" t="b">
-        <v>0</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2016-10-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2016-10-31</t>
+          <t>2016-09-01</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>2016-09-30</t>
         </is>
       </c>
     </row>
@@ -1384,40 +1494,45 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>005_Decreasing_0_190_MoTuWeThFr_2016-12-01_2016-12-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Increasing_0_190_MoTuWeThFr_2016-10-01_2016-10-31.xlsx</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F23" t="b">
-        <v>0</v>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Decreasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2016-12-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2016-12-31</t>
+          <t>2016-10-01</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>2016-10-31</t>
         </is>
       </c>
     </row>
@@ -1427,40 +1542,45 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-07-01_2016-07-31</t>
+          <t>./data/DriveNet/averaged daily data/005_Increasing_0_190_MoTuWeThFr_2016-11-01_2016-11-30.xlsx</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2016-07-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2016-07-31</t>
+          <t>2016-11-01</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>2016-11-30</t>
         </is>
       </c>
     </row>
@@ -1470,40 +1590,45 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>005_Decreasing_0_190_MoTuWeThFr_2016-09-01_2016-09-30</t>
+          <t>./data/DriveNet/averaged daily data/005_Increasing_0_190_MoTuWeThFr_2016-12-01_2016-12-31.xlsx</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>averaged daily data</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Decreasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2016-09-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2016-09-30</t>
+          <t>2016-12-01</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>2016-12-31</t>
         </is>
       </c>
     </row>
@@ -1513,38 +1638,43 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-01-01_2016-01-31</t>
+          <t>./data/DriveNet/daily data/005_Increasing_0_190_MoTuWeThFr_2016-01-01_2016-01-31.xlsx</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>daily data</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
+          <t>Increasing</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
           <t>2016-01-01</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t>2016-01-31</t>
         </is>
@@ -1556,40 +1686,45 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-11-01_2016-11-30</t>
+          <t>./data/DriveNet/daily data/005_Increasing_0_190_MoTuWeThFr_2016-02-01_2016-02-29.xlsx</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>daily data</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F27" t="b">
-        <v>0</v>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2016-11-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2016-11-30</t>
+          <t>2016-02-01</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>2016-02-29</t>
         </is>
       </c>
     </row>
@@ -1599,40 +1734,45 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-06-01_2016-06-30</t>
+          <t>./data/DriveNet/daily data/005_Increasing_0_190_MoTuWeThFr_2016-03-01_2016-03-31.xlsx</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>daily data</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F28" t="b">
-        <v>0</v>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2016-06-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2016-06-30</t>
+          <t>2016-03-01</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>2016-03-31</t>
         </is>
       </c>
     </row>
@@ -1642,40 +1782,45 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-09-01_2016-09-30</t>
+          <t>./data/DriveNet/daily data/005_Increasing_0_190_MoTuWeThFr_2016-04-01_2016-04-30.xlsx</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>daily data</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F29" t="b">
-        <v>0</v>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2016-09-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2016-09-30</t>
+          <t>2016-04-01</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>2016-04-30</t>
         </is>
       </c>
     </row>
@@ -1685,40 +1830,45 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-12-01_2016-12-31</t>
+          <t>./data/DriveNet/daily data/005_Increasing_0_190_MoTuWeThFr_2016-05-01_2016-05-31.xlsx</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>daily data</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F30" t="b">
-        <v>0</v>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2016-12-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2016-12-31</t>
+          <t>2016-05-01</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>2016-05-31</t>
         </is>
       </c>
     </row>
@@ -1728,40 +1878,45 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-05-01_2016-05-31</t>
+          <t>./data/DriveNet/daily data/005_Increasing_0_190_MoTuWeThFr_2016-06-01_2016-06-30.xlsx</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>daily data</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F31" t="b">
-        <v>0</v>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2016-05-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2016-05-31</t>
+          <t>2016-06-01</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>2016-06-30</t>
         </is>
       </c>
     </row>
@@ -1771,36 +1926,45 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>~$005_Increasing_0_190_MoTuWeThFr_2016-06-01_2016-06-30</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr"/>
+          <t>./data/DriveNet/daily data/005_Increasing_0_190_MoTuWeThFr_2016-07-01_2016-07-31.xlsx</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>daily data</t>
+        </is>
+      </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F32" t="b">
-        <v>0</v>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2016-06-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2016-06-30</t>
+          <t>2016-07-01</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>2016-07-31</t>
         </is>
       </c>
     </row>
@@ -1810,40 +1974,45 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-04-01_2016-04-30</t>
+          <t>./data/DriveNet/daily data/005_Increasing_0_190_MoTuWeThFr_2016-08-01_2016-08-31.xlsx</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>daily data</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F33" t="b">
-        <v>0</v>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2016-04-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2016-04-30</t>
+          <t>2016-08-01</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>2016-08-31</t>
         </is>
       </c>
     </row>
@@ -1853,40 +2022,45 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-02-01_2016-02-29</t>
+          <t>./data/DriveNet/daily data/005_Increasing_0_190_MoTuWeThFr_2016-09-01_2016-09-30.xlsx</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>daily data</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F34" t="b">
-        <v>0</v>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2016-02-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2016-02-29</t>
+          <t>2016-09-01</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>2016-09-30</t>
         </is>
       </c>
     </row>
@@ -1896,40 +2070,45 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-03-01_2016-03-31</t>
+          <t>./data/DriveNet/daily data/005_Increasing_0_190_MoTuWeThFr_2016-10-01_2016-10-31.xlsx</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>daily data</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F35" t="b">
-        <v>0</v>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2016-03-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2016-03-31</t>
+          <t>2016-10-01</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>2016-10-31</t>
         </is>
       </c>
     </row>
@@ -1939,40 +2118,45 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-08-01_2016-08-31</t>
+          <t>./data/DriveNet/daily data/005_Increasing_0_190_MoTuWeThFr_2016-11-01_2016-11-30.xlsx</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>daily data</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F36" t="b">
-        <v>0</v>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2016-08-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2016-08-31</t>
+          <t>2016-11-01</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>2016-11-30</t>
         </is>
       </c>
     </row>
@@ -1982,83 +2166,45 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-10-01_2016-10-31</t>
+          <t>./data/DriveNet/daily data/005_Increasing_0_190_MoTuWeThFr_2016-12-01_2016-12-31.xlsx</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>daily data</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F37" t="b">
-        <v>0</v>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2016-10-01</t>
+          <t>Increasing</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2016-10-31</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>005_Increasing_0_190_MoTuWeThFr_2016-07-01_2016-07-31</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>I5</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>190</t>
-        </is>
-      </c>
-      <c r="F38" t="b">
-        <v>0</v>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Increasing</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>2016-07-01</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>2016-07-31</t>
+          <t>2016-12-01</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>2016-12-31</t>
         </is>
       </c>
     </row>

</xml_diff>